<commit_message>
updates to roster cells
</commit_message>
<xml_diff>
--- a/roster.xlsx
+++ b/roster.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khuynh46/Library/CloudStorage/OneDrive-GeorgiaInstituteofTechnology/Documents/RA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CA2B64-056F-F041-B924-225EAA33B38C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489C3212-8208-1D43-A4D0-F4D08A7C4962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5740" yWindow="0" windowWidth="23060" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -449,7 +449,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -458,10 +458,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -474,6 +474,327 @@
   </cellStyles>
   <dxfs count="27">
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
@@ -486,327 +807,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <fill>
@@ -872,28 +872,28 @@
   <tableColumns count="25">
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Column4"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Column5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Column6" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Column7" dataDxfId="0"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Column8" dataDxfId="21"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Column9" dataDxfId="20"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Column10" dataDxfId="19"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Column11" dataDxfId="18"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Column12" dataDxfId="17"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Column13" dataDxfId="16"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Column14" dataDxfId="15"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Column15" dataDxfId="14"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Column16" dataDxfId="13"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Column17" dataDxfId="12"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Column18" dataDxfId="11"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Column19" dataDxfId="10"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Column20" dataDxfId="9"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Column21" dataDxfId="8"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Column22" dataDxfId="7"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Column23" dataDxfId="6"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Column24" dataDxfId="5"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Column25" dataDxfId="4"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Column26" dataDxfId="3"/>
-    <tableColumn id="1" xr3:uid="{E8DCCF55-BEDC-5548-97B0-2DDA9B33C321}" name="Column1" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Column6" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Column7" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Column8" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Column9" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Column10" dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Column11" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Column12" dataDxfId="15"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Column13" dataDxfId="14"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Column14" dataDxfId="13"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Column15" dataDxfId="12"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Column16" dataDxfId="11"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Column17" dataDxfId="10"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Column18" dataDxfId="9"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Column19" dataDxfId="8"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Column20" dataDxfId="7"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Column21" dataDxfId="6"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Column22" dataDxfId="5"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Column23" dataDxfId="4"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Column24" dataDxfId="3"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Column25" dataDxfId="2"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Column26" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{E8DCCF55-BEDC-5548-97B0-2DDA9B33C321}" name="Column1" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{0B397F88-DA85-244E-B7F5-AA8171BED77C}" name="Column2"/>
   </tableColumns>
   <tableStyleInfo name="Sheet1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="1"/>

</xml_diff>